<commit_message>
ajustes generales de clientes y migracion
</commit_message>
<xml_diff>
--- a/migracion/reporte_migracion.xlsx
+++ b/migracion/reporte_migracion.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G179"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -508,7 +508,7 @@
         <v>153</v>
       </c>
       <c r="E5">
-        <v>967</v>
+        <v>1002</v>
       </c>
       <c r="F5" t="str">
         <v>OK</v>
@@ -686,13 +686,13 @@
         <v>900654612</v>
       </c>
       <c r="C13">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D13">
         <v>67</v>
       </c>
       <c r="E13">
-        <v>874</v>
+        <v>914</v>
       </c>
       <c r="F13" t="str">
         <v>OK</v>
@@ -758,10 +758,10 @@
         <v>11</v>
       </c>
       <c r="D16">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F16" t="str">
         <v>OK</v>
@@ -968,7 +968,7 @@
         <v>162</v>
       </c>
       <c r="E25">
-        <v>2832</v>
+        <v>2919</v>
       </c>
       <c r="F25" t="str">
         <v>OK</v>
@@ -1336,7 +1336,7 @@
         <v>21</v>
       </c>
       <c r="E41">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="F41" t="str">
         <v>OK</v>
@@ -1451,7 +1451,7 @@
         <v>14</v>
       </c>
       <c r="E46">
-        <v>479</v>
+        <v>498</v>
       </c>
       <c r="F46" t="str">
         <v>OK</v>
@@ -1497,7 +1497,7 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F48" t="str">
         <v>OK</v>
@@ -1658,7 +1658,7 @@
         <v>99</v>
       </c>
       <c r="E55">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="F55" t="str">
         <v>OK</v>
@@ -1727,7 +1727,7 @@
         <v>44</v>
       </c>
       <c r="E58">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="F58" t="str">
         <v>OK</v>
@@ -1934,7 +1934,7 @@
         <v>31</v>
       </c>
       <c r="E67">
-        <v>551</v>
+        <v>565</v>
       </c>
       <c r="F67" t="str">
         <v>OK</v>
@@ -2463,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="E90">
-        <v>436</v>
+        <v>479</v>
       </c>
       <c r="F90" t="str">
         <v>OK</v>
@@ -2670,7 +2670,7 @@
         <v>16</v>
       </c>
       <c r="E99">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="F99" t="str">
         <v>OK</v>
@@ -2762,7 +2762,7 @@
         <v>177</v>
       </c>
       <c r="E103">
-        <v>2403</v>
+        <v>2433</v>
       </c>
       <c r="F103" t="str">
         <v>OK</v>
@@ -2785,7 +2785,7 @@
         <v>44</v>
       </c>
       <c r="E104">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="F104" t="str">
         <v>OK</v>
@@ -3107,7 +3107,7 @@
         <v>160</v>
       </c>
       <c r="E118">
-        <v>1140</v>
+        <v>1175</v>
       </c>
       <c r="F118" t="str">
         <v>OK</v>
@@ -3130,7 +3130,7 @@
         <v>17</v>
       </c>
       <c r="E119">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="F119" t="str">
         <v>OK</v>
@@ -3196,10 +3196,10 @@
         <v>34</v>
       </c>
       <c r="D122">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E122">
-        <v>502</v>
+        <v>531</v>
       </c>
       <c r="F122" t="str">
         <v>OK</v>
@@ -3219,10 +3219,10 @@
         <v>59</v>
       </c>
       <c r="D123">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E123">
-        <v>1431</v>
+        <v>1456</v>
       </c>
       <c r="F123" t="str">
         <v>OK</v>
@@ -3360,7 +3360,7 @@
         <v>10</v>
       </c>
       <c r="E129">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="F129" t="str">
         <v>OK</v>
@@ -3383,7 +3383,7 @@
         <v>21</v>
       </c>
       <c r="E130">
-        <v>545</v>
+        <v>557</v>
       </c>
       <c r="F130" t="str">
         <v>OK</v>
@@ -3866,7 +3866,7 @@
         <v>91</v>
       </c>
       <c r="E151">
-        <v>763</v>
+        <v>775</v>
       </c>
       <c r="F151" t="str">
         <v>OK</v>
@@ -4303,7 +4303,7 @@
         <v>70</v>
       </c>
       <c r="E170">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="F170" t="str">
         <v>OK</v>
@@ -4326,7 +4326,7 @@
         <v>20</v>
       </c>
       <c r="E171">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F171" t="str">
         <v>OK</v>
@@ -4519,9 +4519,32 @@
         <v/>
       </c>
     </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>CONJUNTO MAZUREN SECTOR II AGRUPACION 3 - P.H.</v>
+      </c>
+      <c r="B180" t="str">
+        <v>830135053</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180" t="str">
+        <v>NO ESTA EN NOMOS</v>
+      </c>
+      <c r="G180" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G179"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G180"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>